<commit_message>
US City updates with figures
</commit_message>
<xml_diff>
--- a/data/input_data_US_group1.xlsx
+++ b/data/input_data_US_group1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom.walsh\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1352A44F-C552-43A6-915D-3DB9DF394117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2544FD-404E-4ECA-A824-187A758B6F98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1770" yWindow="3105" windowWidth="14745" windowHeight="7815" tabRatio="839" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-7380" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_sex" sheetId="1" r:id="rId1"/>
@@ -943,9 +943,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -953,6 +950,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1919,7 +1919,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="63" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="40" t="s">
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="40" t="s">
         <v>20</v>
       </c>
@@ -2037,7 +2037,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="61" t="s">
         <v>101</v>
       </c>
       <c r="B12" s="41" t="s">
@@ -2097,7 +2097,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="41" t="s">
         <v>20</v>
       </c>
@@ -2155,7 +2155,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="64" t="s">
         <v>102</v>
       </c>
       <c r="B14" s="56" t="s">
@@ -2216,7 +2216,7 @@
       <c r="T14" s="42"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="56" t="s">
         <v>20</v>
       </c>
@@ -2277,7 +2277,7 @@
       <c r="U15" s="42"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="64" t="s">
         <v>103</v>
       </c>
       <c r="B16" s="57" t="s">
@@ -2338,7 +2338,7 @@
       <c r="T16" s="59"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="57" t="s">
         <v>20</v>
       </c>
@@ -2398,7 +2398,7 @@
       <c r="U17" s="42"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="64" t="s">
         <v>104</v>
       </c>
       <c r="B18" s="58" t="s">
@@ -2459,7 +2459,7 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="58" t="s">
         <v>20</v>
       </c>
@@ -3028,7 +3028,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="46" t="s">
         <v>21</v>
       </c>
@@ -3085,7 +3085,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="64" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="46" t="s">
@@ -3161,7 +3161,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="46" t="s">
         <v>21</v>
       </c>
@@ -3235,7 +3235,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="61" t="s">
+      <c r="A30" s="64" t="s">
         <v>101</v>
       </c>
       <c r="B30" s="46" t="s">
@@ -3311,7 +3311,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="46" t="s">
         <v>21</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="61" t="s">
+      <c r="A32" s="64" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="46" t="s">
@@ -3461,7 +3461,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="46" t="s">
         <v>21</v>
       </c>
@@ -3535,7 +3535,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="64" t="s">
         <v>103</v>
       </c>
       <c r="B34" s="46" t="s">
@@ -3612,7 +3612,7 @@
       <c r="T34" s="42"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="61"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="46" t="s">
         <v>21</v>
       </c>
@@ -3688,7 +3688,7 @@
       <c r="U35" s="42"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="61" t="s">
+      <c r="A36" s="64" t="s">
         <v>104</v>
       </c>
       <c r="B36" s="46" t="s">
@@ -3765,7 +3765,7 @@
       <c r="T36" s="42"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="61"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="46" t="s">
         <v>21</v>
       </c>
@@ -3932,14 +3932,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A15"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
@@ -3950,6 +3942,14 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38837,8 +38837,8 @@
   </sheetPr>
   <dimension ref="A1:N255"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38855,8 +38855,8 @@
     <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -41051,7 +41051,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41059,14 +41059,16 @@
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="24" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="14" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="24" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" customWidth="1"/>
     <col min="17" max="17" width="13.140625" customWidth="1"/>
     <col min="18" max="18" width="9.5703125" customWidth="1"/>
@@ -41270,7 +41272,7 @@
         <v>120</v>
       </c>
       <c r="Q3">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="R3">
         <v>1000</v>
@@ -41702,7 +41704,7 @@
         <v>150</v>
       </c>
       <c r="Q9">
-        <v>5500</v>
+        <v>5000</v>
       </c>
       <c r="R9">
         <v>4500</v>

</xml_diff>